<commit_message>
Added tree drawing for linear program
</commit_message>
<xml_diff>
--- a/tree_prototype.xlsx
+++ b/tree_prototype.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\GitHub\Graph-Drawing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F1FA72A-7BBA-49E5-9A2C-CEB829997A88}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B90EC0-92AC-4300-AD28-1C1E7F1A6B0F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{E0DB2D5E-48DA-4757-89CB-BCB2CBD85693}"/>
   </bookViews>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26513369-1214-4673-9889-8B6D2B5B822D}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -592,7 +592,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
@@ -636,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>